<commit_message>
add distributor master page
</commit_message>
<xml_diff>
--- a/Excel_TestData/Excel_Havmor.xlsx
+++ b/Excel_TestData/Excel_Havmor.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="5112" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Distributor_Add" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:Q15"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Username</t>
   </si>
@@ -29,16 +31,81 @@
   </si>
   <si>
     <t>Heera@11</t>
+  </si>
+  <si>
+    <t>Distributor Code</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Contact Person name</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>Address3</t>
+  </si>
+  <si>
+    <t>Pin Code</t>
+  </si>
+  <si>
+    <t>Pan Number</t>
+  </si>
+  <si>
+    <t>FSSAI Licence number</t>
+  </si>
+  <si>
+    <t>DB5102</t>
+  </si>
+  <si>
+    <t>Aniket Enterprices</t>
+  </si>
+  <si>
+    <t>Aniket sharma</t>
+  </si>
+  <si>
+    <t>aniket.jadhav@heerasoftware.com</t>
+  </si>
+  <si>
+    <t>krudhani sahara appartment</t>
+  </si>
+  <si>
+    <t>washing center</t>
+  </si>
+  <si>
+    <t>mumbai</t>
+  </si>
+  <si>
+    <t>KOPGF5479U</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -61,13 +128,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -372,7 +443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -407,4 +478,102 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="30.21875" customWidth="1"/>
+    <col min="6" max="6" width="24.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" customWidth="1"/>
+    <col min="11" max="11" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>9457863214</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2">
+        <v>400701</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2">
+        <v>10017022012345</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add new files 10
</commit_message>
<xml_diff>
--- a/Excel_TestData/Excel_Havmor.xlsx
+++ b/Excel_TestData/Excel_Havmor.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="5112" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Distributor_Add" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:Q15"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Username</t>
   </si>
@@ -29,16 +31,81 @@
   </si>
   <si>
     <t>Heera@11</t>
+  </si>
+  <si>
+    <t>Distributor Code</t>
+  </si>
+  <si>
+    <t>Distributor Name</t>
+  </si>
+  <si>
+    <t>Contact person name</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>Address3</t>
+  </si>
+  <si>
+    <t>PinCode</t>
+  </si>
+  <si>
+    <t>Pan Number</t>
+  </si>
+  <si>
+    <t>FSSAI Licence Number</t>
+  </si>
+  <si>
+    <t>DB5410</t>
+  </si>
+  <si>
+    <t>Aditya</t>
+  </si>
+  <si>
+    <t>Aditya Thakur</t>
+  </si>
+  <si>
+    <t>aniket.jadhav@heerasoftware.com</t>
+  </si>
+  <si>
+    <t>ramai nagar</t>
+  </si>
+  <si>
+    <t>washing center</t>
+  </si>
+  <si>
+    <t>narhe</t>
+  </si>
+  <si>
+    <t>POYTF5487K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -61,13 +128,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -372,7 +442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -407,4 +477,103 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="29.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>9654862012</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2">
+        <v>441611</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2">
+        <v>10012022001234</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New changes  11 sept
</commit_message>
<xml_diff>
--- a/Excel_TestData/Excel_Havmor.xlsx
+++ b/Excel_TestData/Excel_Havmor.xlsx
@@ -3,20 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04900757-F4E1-463D-9E12-390142BB3FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40BEBE7-EF1A-44E6-9CA5-B8E97F1FEC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Route_Add" sheetId="2" r:id="rId2"/>
+    <sheet name="Distributor_Add" sheetId="3" r:id="rId2"/>
+    <sheet name="Route_Add" sheetId="2" r:id="rId3"/>
+    <sheet name="Salesman_Add" sheetId="4" r:id="rId4"/>
+    <sheet name="User_Master_ADD" sheetId="5" r:id="rId5"/>
+    <sheet name="Retailer_Add" sheetId="6" r:id="rId6"/>
+    <sheet name="Vendor_Add" sheetId="7" r:id="rId7"/>
+    <sheet name="Depot_Add" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="95">
   <si>
     <t>Username</t>
   </si>
@@ -34,16 +40,298 @@
   </si>
   <si>
     <t>Karve Nagar</t>
+  </si>
+  <si>
+    <t>Distributor Code</t>
+  </si>
+  <si>
+    <t>Distributor Name</t>
+  </si>
+  <si>
+    <t>Contact person name</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>Address3</t>
+  </si>
+  <si>
+    <t>PinCode</t>
+  </si>
+  <si>
+    <t>Pan Number</t>
+  </si>
+  <si>
+    <t>FSSAI Licence Number</t>
+  </si>
+  <si>
+    <t>DB5410</t>
+  </si>
+  <si>
+    <t>Aditya</t>
+  </si>
+  <si>
+    <t>Aditya Thakur</t>
+  </si>
+  <si>
+    <t>aniket.jadhav@heerasoftware.com</t>
+  </si>
+  <si>
+    <t>ramai nagar</t>
+  </si>
+  <si>
+    <t>washing center</t>
+  </si>
+  <si>
+    <t>narhe</t>
+  </si>
+  <si>
+    <t>POYTF5487K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee Code/UserId </t>
+  </si>
+  <si>
+    <t>Salesman Name</t>
+  </si>
+  <si>
+    <t>Address 1 </t>
+  </si>
+  <si>
+    <t>Pincode</t>
+  </si>
+  <si>
+    <t>Email_ID</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Adhar</t>
+  </si>
+  <si>
+    <t>Pan No</t>
+  </si>
+  <si>
+    <t>Bank Number</t>
+  </si>
+  <si>
+    <t>Account Holder Name</t>
+  </si>
+  <si>
+    <t>Bank IFSC Code</t>
+  </si>
+  <si>
+    <t>Branch Name</t>
+  </si>
+  <si>
+    <t>Salary Contribution</t>
+  </si>
+  <si>
+    <t>Distributor Contribution</t>
+  </si>
+  <si>
+    <t>Company Contribution</t>
+  </si>
+  <si>
+    <t>P1001380495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mukesh SING </t>
+  </si>
+  <si>
+    <t>SHOP NO. 12 GROUND FLOOR Gulab shilp</t>
+  </si>
+  <si>
+    <t>roshan.zambare@heerasoftware.com</t>
+  </si>
+  <si>
+    <t>PQRSX6789L</t>
+  </si>
+  <si>
+    <t>SBIN0001234</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>User ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile </t>
+  </si>
+  <si>
+    <t>Retailer Firm Name</t>
+  </si>
+  <si>
+    <t>ERP Code</t>
+  </si>
+  <si>
+    <t>Address Line 1</t>
+  </si>
+  <si>
+    <t>Land Mark</t>
+  </si>
+  <si>
+    <t>Contact Person Name</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>PAN Number</t>
+  </si>
+  <si>
+    <t>Potencial Business</t>
+  </si>
+  <si>
+    <t>GST Number</t>
+  </si>
+  <si>
+    <t>Food Licence number</t>
+  </si>
+  <si>
+    <t>Expiery Date</t>
+  </si>
+  <si>
+    <t>Bank Account number</t>
+  </si>
+  <si>
+    <t>Pitamber dairy</t>
+  </si>
+  <si>
+    <t>G1001</t>
+  </si>
+  <si>
+    <t>indora square</t>
+  </si>
+  <si>
+    <t>pitamber kamble</t>
+  </si>
+  <si>
+    <t>PHSYB6579U</t>
+  </si>
+  <si>
+    <t>09AAACH7409R1ZZ</t>
+  </si>
+  <si>
+    <t>25/10/2025</t>
+  </si>
+  <si>
+    <t>ABHY0065107</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>Vendor Name</t>
+  </si>
+  <si>
+    <t>Vendor ID From ERP</t>
+  </si>
+  <si>
+    <t>Email ID</t>
+  </si>
+  <si>
+    <t>GST No</t>
+  </si>
+  <si>
+    <t>VM1012</t>
+  </si>
+  <si>
+    <t>Yash Thakur</t>
+  </si>
+  <si>
+    <t>VND00123</t>
+  </si>
+  <si>
+    <t>Maya Nagar</t>
+  </si>
+  <si>
+    <t>Narhe</t>
+  </si>
+  <si>
+    <t>Depot Code</t>
+  </si>
+  <si>
+    <t>Depot Name</t>
+  </si>
+  <si>
+    <t>Emai ID</t>
+  </si>
+  <si>
+    <t>Mobile No</t>
+  </si>
+  <si>
+    <t>FSSAI Expiry Date</t>
+  </si>
+  <si>
+    <t>D51246</t>
+  </si>
+  <si>
+    <t>Aniket Enterprices</t>
+  </si>
+  <si>
+    <t>Aniket Thakur</t>
+  </si>
+  <si>
+    <t>DM1012</t>
+  </si>
+  <si>
+    <t>civil lines</t>
+  </si>
+  <si>
+    <t>Route Name</t>
+  </si>
+  <si>
+    <t>P1001380496</t>
+  </si>
+  <si>
+    <t>Amit Kadtan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -57,7 +345,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -65,14 +353,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -415,18 +743,573 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64544C8D-F492-4A3C-91E6-D7886F11C0BB}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC8A147-90D9-4E04-A66B-3D99799900AE}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9654862012</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="1">
+        <v>441611</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="3">
+        <v>10012000000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" tooltip="mailto:aniket.jadhav@heerasoftware.com" display="mailto:aniket.jadhav@heerasoftware.com" xr:uid="{23590D03-93BB-41E7-BD35-0E9C4E015825}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64544C8D-F492-4A3C-91E6-D7886F11C0BB}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F6A36E-6FE1-4342-A759-9C792F096782}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="24" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" customWidth="1"/>
+    <col min="14" max="14" width="24.42578125" customWidth="1"/>
+    <col min="15" max="15" width="28.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="7">
+        <v>411009</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="7">
+        <v>9667774565</v>
+      </c>
+      <c r="G2" s="11">
+        <v>757567567567</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="11">
+        <v>897979879879879</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="7">
+        <v>100</v>
+      </c>
+      <c r="N2" s="7">
+        <v>70</v>
+      </c>
+      <c r="O2" s="7">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{DDFF0FD4-555C-4429-9AFC-D4E84835F998}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909E620E-9E59-486E-9771-017302C48C14}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="7">
+        <v>9667774565</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{5F319C3B-F169-46F6-8CFF-7054F8D65BFE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E21A26D-DB81-4E85-A562-A8AB1FB3FABD}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="4">
+        <v>411041</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="4">
+        <v>9865470215</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="6">
+        <v>34186</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="4">
+        <v>350</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2" s="4">
+        <v>678987678987689</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="O2" s="4">
+        <v>234567890987654</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" tooltip="mailto:aniket.jadhav@heerasoftware.com" display="mailto:aniket.jadhav@heerasoftware.com" xr:uid="{4C4C8ACE-BA60-4234-B3B0-41F607E9EA33}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF86D4CF-74CB-4177-89A3-EDE059EEA1EF}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="4">
+        <v>9865124780</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="4">
+        <v>411041</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" tooltip="mailto:aniket.jadhav@heerasoftware.com" display="mailto:aniket.jadhav@heerasoftware.com" xr:uid="{AC4388A9-669A-4B53-B85D-6721AB431B7D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D5F150-07FA-494D-9F76-1F8D7F8CE447}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="4">
+        <v>9657841203</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="4">
+        <v>412012</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="4">
+        <v>10012022001234</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Retailer Jenkins Run"
</commit_message>
<xml_diff>
--- a/Excel_TestData/Excel_Havmor.xlsx
+++ b/Excel_TestData/Excel_Havmor.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA13C8DD-9E20-4401-846B-564F8B639BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB6749A-FDDF-4A17-A446-E66DDBD74841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7785" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="96">
   <si>
     <t>Username</t>
   </si>
@@ -247,6 +247,9 @@
     <t>roshan.zambare@heerasoftware.com</t>
   </si>
   <si>
+    <t>Employee Code/UserId</t>
+  </si>
+  <si>
     <t>Salesman Name</t>
   </si>
   <si>
@@ -308,15 +311,6 @@
   </si>
   <si>
     <t>Raj Thakur</t>
-  </si>
-  <si>
-    <t>UserId</t>
-  </si>
-  <si>
-    <t>Employee Code</t>
-  </si>
-  <si>
-    <t>SM101</t>
   </si>
 </sst>
 </file>
@@ -1200,135 +1194,128 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="38.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="39.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1"/>
-    <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" customWidth="1"/>
-    <col min="16" max="16" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>96</v>
+    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
         <v>87</v>
       </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>88</v>
+      </c>
       <c r="B2" s="7" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="7">
+        <v>411009</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="7">
+        <v>9667774565</v>
+      </c>
+      <c r="G2" s="9">
+        <v>757567567567</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="7">
-        <v>411009</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="7">
-        <v>9667774565</v>
-      </c>
-      <c r="H2" s="9">
-        <v>757567567567</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="K2" s="10">
+      <c r="J2" s="10">
         <v>897979879879879</v>
       </c>
+      <c r="K2" s="7" t="s">
+        <v>92</v>
+      </c>
       <c r="L2" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+      <c r="M2" s="7">
+        <v>100</v>
       </c>
       <c r="N2" s="7">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="O2" s="7">
-        <v>70</v>
-      </c>
-      <c r="P2" s="7">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" tooltip="mailto:roshan.zambare@heerasoftware.com" display="mailto:roshan.zambare@heerasoftware.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId1" tooltip="mailto:roshan.zambare@heerasoftware.com" display="mailto:roshan.zambare@heerasoftware.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1391,7 +1378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1402,12 +1389,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>